<commit_message>
Usar Trend (pendiente de los últimos 3 días) capturó dinámicas locales del precio.
Split aleatorio (train_test_split) permitió al modelo ver varios tipos de comportamientos históricos, no solo una tendencia lineal.

100 árboles en el bosque lo hicieron más robusto.

random_state nos da reproducibilidad: podés volver a obtener estos resultados si lo volvés a ejecutar
</commit_message>
<xml_diff>
--- a/proyecto_dolardjango/USD_ARSB_Diario_2016_2023_mod.xlsx
+++ b/proyecto_dolardjango/USD_ARSB_Diario_2016_2023_mod.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kochl\OneDrive\Escritorio\Proyecto_dolar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kochl\OneDrive\Escritorio\dolardjango\proyecto_dolardjango\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7AC6EC-847A-4C67-B578-579DA109D51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F77149-6441-4272-A537-77A65E593D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4050" yWindow="5430" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USD_ARSB_Diario_2016_2023_mod" sheetId="1" r:id="rId1"/>
@@ -881,7 +881,7 @@
   <dimension ref="A1:E1916"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" activeCellId="5" sqref="C2:C1048576 D2:D1048576 E2:E1048576 B3:B1048576 B2 F4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>